<commit_message>
Add Consumer data base file
</commit_message>
<xml_diff>
--- a/Consumer_DATA_BASE.xlsx
+++ b/Consumer_DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22296864-4A61-4A7C-BEBD-837877B157B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486AE06A-BB02-4964-8CE0-0C8097FDE58F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SoC" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
@@ -1311,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57046388-826A-44FA-9732-DCABAA83AE86}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New features for the new consumer database to be functional
</commit_message>
<xml_diff>
--- a/Consumer_DATA_BASE.xlsx
+++ b/Consumer_DATA_BASE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33341A0-E741-4B13-8D5C-69B45DFD6B95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016079F5-B3D0-46C3-95DC-C9C6AE0ACB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SoC" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="DDR" sheetId="3" r:id="rId3"/>
     <sheet name="PHY" sheetId="4" r:id="rId4"/>
     <sheet name="WIFI" sheetId="5" r:id="rId5"/>
-    <sheet name="USB" sheetId="7" r:id="rId6"/>
-    <sheet name="HDMI" sheetId="8" r:id="rId7"/>
+    <sheet name="Front End" sheetId="9" r:id="rId6"/>
+    <sheet name="USB" sheetId="7" r:id="rId7"/>
+    <sheet name="HDMI" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="64">
   <si>
     <t>SoC</t>
   </si>
@@ -93,12 +94,6 @@
     <t>Current peak</t>
   </si>
   <si>
-    <t>eMMC</t>
-  </si>
-  <si>
-    <t>16GB</t>
-  </si>
-  <si>
     <t>Vcc</t>
   </si>
   <si>
@@ -111,21 +106,12 @@
     <t>I max mesure</t>
   </si>
   <si>
-    <t>LpDDR4</t>
-  </si>
-  <si>
     <t>Obligatoire</t>
   </si>
   <si>
     <t>Facultatif</t>
   </si>
   <si>
-    <t>MICRON 3GB</t>
-  </si>
-  <si>
-    <t>MT53E768M32</t>
-  </si>
-  <si>
     <t>VDDQ 1V1</t>
   </si>
   <si>
@@ -163,6 +149,81 @@
   </si>
   <si>
     <t>I théorique</t>
+  </si>
+  <si>
+    <t>Fabricant</t>
+  </si>
+  <si>
+    <t>AMLogic</t>
+  </si>
+  <si>
+    <t>SDINBDG4-16G-1231T</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>eMMC 16GB</t>
+  </si>
+  <si>
+    <t>SANDISK</t>
+  </si>
+  <si>
+    <t>LpDDR4 3GB</t>
+  </si>
+  <si>
+    <t>Realteck</t>
+  </si>
+  <si>
+    <t>SKY85207</t>
+  </si>
+  <si>
+    <t>QPF4506BSR</t>
+  </si>
+  <si>
+    <t>PA 5G</t>
+  </si>
+  <si>
+    <t>PA 2G</t>
+  </si>
+  <si>
+    <t>SKYWORKS</t>
+  </si>
+  <si>
+    <t>QORVO</t>
+  </si>
+  <si>
+    <t>H26M52208FPR</t>
+  </si>
+  <si>
+    <t>SK HYNIX</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>LpDDR4x 2GB</t>
+  </si>
+  <si>
+    <t>VDDQ</t>
+  </si>
+  <si>
+    <t>VDD1</t>
+  </si>
+  <si>
+    <t>VDD2</t>
+  </si>
+  <si>
+    <t>191494614-xx</t>
+  </si>
+  <si>
+    <t>191687123-xx</t>
+  </si>
+  <si>
+    <t>K4FHE3D4HM-MGCJ - DIE M</t>
+  </si>
+  <si>
+    <t>K4U6E3S4AB-MGCL - DIE B</t>
   </si>
 </sst>
 </file>
@@ -224,7 +285,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,15 +570,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
@@ -527,12 +590,12 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -545,13 +608,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -562,6 +625,9 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2">
@@ -586,7 +652,7 @@
         <v>510</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -594,6 +660,9 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2">
@@ -618,7 +687,7 @@
         <v>2300</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -626,6 +695,9 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2">
@@ -646,6 +718,9 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2">
@@ -666,6 +741,9 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2">
@@ -686,6 +764,9 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2">
@@ -706,6 +787,9 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2">
@@ -726,6 +810,9 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="2">
@@ -746,6 +833,9 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2">
@@ -766,6 +856,9 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2">
@@ -786,6 +879,9 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2">
@@ -806,6 +902,9 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="2">
@@ -828,17 +927,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14682EF4-3407-4104-BC07-495A063FFEE7}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="2"/>
-    <col min="3" max="3" width="11.42578125" style="4"/>
-    <col min="4" max="7" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" style="2"/>
     <col min="8" max="8" width="16.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="14" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
@@ -846,12 +947,12 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -864,13 +965,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -878,16 +979,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>191484457</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2">
         <v>3.3</v>
@@ -896,21 +1000,24 @@
         <v>60</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>191484457</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>1.8</v>
@@ -928,7 +1035,53 @@
         <v>330</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2">
+        <v>191401325</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="2">
+        <v>191401325</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -938,18 +1091,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACFB5E0-D019-4CA8-AD55-42E505099734}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="13" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="2"/>
+    <col min="3" max="3" width="27.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="2"/>
     <col min="7" max="7" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -957,12 +1111,12 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -975,13 +1129,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -989,60 +1143,123 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="2">
-        <v>191435694</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="G2" s="2">
-        <v>380</v>
+        <v>253</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2">
-        <v>191435694</v>
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2">
         <v>1.8</v>
       </c>
       <c r="G3" s="2">
-        <v>40</v>
-      </c>
-      <c r="H3" s="3">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1055,14 +1272,14 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11.42578125" style="2"/>
     <col min="7" max="7" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -1074,9 +1291,9 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1089,13 +1306,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -1103,16 +1320,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="2">
         <v>191616666</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2">
         <v>3.3</v>
@@ -1123,12 +1343,12 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="O4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1141,14 +1361,14 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2"/>
     <col min="2" max="2" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11.42578125" style="2"/>
     <col min="7" max="7" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -1160,9 +1380,9 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1175,13 +1395,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -1189,16 +1409,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="D2" s="2">
         <v>191653239</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2">
         <v>3.3</v>
@@ -1217,13 +1440,55 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2">
+        <v>191479021</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>221</v>
+      </c>
       <c r="O3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2">
+        <v>191479034</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>221</v>
+      </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1232,11 +1497,77 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB425FF-3332-4B83-850F-FF6DC8D2F6D9}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="2" customWidth="1"/>
+    <col min="4" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="16.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEE10A5-F188-4041-A5FD-DA2E8FF4B590}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,9 +1586,9 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1270,13 +1601,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -1284,16 +1615,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2">
         <v>5</v>
@@ -1307,12 +1638,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57046388-826A-44FA-9732-DCABAA83AE86}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,9 +1662,9 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1346,13 +1677,13 @@
         <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>19</v>
@@ -1363,13 +1694,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2">
         <v>3.3</v>

</xml_diff>

<commit_message>
Debug link dcdc/consumer -> OK
</commit_message>
<xml_diff>
--- a/Consumer_DATA_BASE.xlsx
+++ b/Consumer_DATA_BASE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016079F5-B3D0-46C3-95DC-C9C6AE0ACB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF2C10-5538-4617-8E2B-F21310B7FA19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>